<commit_message>
new functions to clean input data
</commit_message>
<xml_diff>
--- a/data/output/Anfragen_Geschenk_Muster_Spendende_Beispiele.xlsx
+++ b/data/output/Anfragen_Geschenk_Muster_Spendende_Beispiele.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="70">
   <si>
     <t>Titel</t>
   </si>
@@ -31,18 +31,18 @@
     <t>ISBN</t>
   </si>
   <si>
+    <t>nach_ISBN_Titel</t>
+  </si>
+  <si>
+    <t>nach_ISBN_Sprache_Text</t>
+  </si>
+  <si>
+    <t>Verlag</t>
+  </si>
+  <si>
     <t>Erscheinungsort</t>
   </si>
   <si>
-    <t>Verlag</t>
-  </si>
-  <si>
-    <t>nach_ISBN_Titel</t>
-  </si>
-  <si>
-    <t>nach_ISBN_Sprache_Text</t>
-  </si>
-  <si>
     <t>nach_ISBN_Bestand_K10</t>
   </si>
   <si>
@@ -97,57 +97,18 @@
     <t>La familia de Pascual Duarte</t>
   </si>
   <si>
-    <t>Auf der Eidechsburg</t>
-  </si>
-  <si>
-    <t>Bayerisches Kochbuch</t>
-  </si>
-  <si>
-    <t>Centenaire de l‘Impressionisme</t>
-  </si>
-  <si>
-    <t>Les parents terribles</t>
-  </si>
-  <si>
-    <t>Straightforward Statistics</t>
-  </si>
-  <si>
     <t>Oscar</t>
   </si>
   <si>
     <t>Camilo José</t>
   </si>
   <si>
-    <t>Ilse-Dore</t>
-  </si>
-  <si>
-    <t>Maria</t>
-  </si>
-  <si>
-    <t>Jean</t>
-  </si>
-  <si>
-    <t>James D.</t>
-  </si>
-  <si>
     <t>Wilde</t>
   </si>
   <si>
     <t>Cela</t>
   </si>
   <si>
-    <t>Tanner</t>
-  </si>
-  <si>
-    <t>Hofmann</t>
-  </si>
-  <si>
-    <t>Cocteau</t>
-  </si>
-  <si>
-    <t>Evans</t>
-  </si>
-  <si>
     <t>1994</t>
   </si>
   <si>
@@ -157,9 +118,6 @@
     <t>2009</t>
   </si>
   <si>
-    <t>1938?</t>
-  </si>
-  <si>
     <t>9780140623222</t>
   </si>
   <si>
@@ -169,69 +127,42 @@
     <t>9788423339044</t>
   </si>
   <si>
+    <t>The @picture of Dorian Gray</t>
+  </si>
+  <si>
+    <t>Gustav Klimt - Art Nouveau visionary</t>
+  </si>
+  <si>
+    <t>La @familia de Pascual Duarte</t>
+  </si>
+  <si>
+    <t>eng</t>
+  </si>
+  <si>
+    <t>spa</t>
+  </si>
+  <si>
+    <t>Penguin Books</t>
+  </si>
+  <si>
+    <t>Sterling</t>
+  </si>
+  <si>
+    <t>Ed. Destino</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>New York [u.a.]</t>
+  </si>
+  <si>
+    <t>Barcelona</t>
+  </si>
+  <si>
     <t>0</t>
   </si>
   <si>
-    <t>London</t>
-  </si>
-  <si>
-    <t>New York [u.a.]</t>
-  </si>
-  <si>
-    <t>Barcelona</t>
-  </si>
-  <si>
-    <t>Leipzig</t>
-  </si>
-  <si>
-    <t>München</t>
-  </si>
-  <si>
-    <t>Paris</t>
-  </si>
-  <si>
-    <t>Pacific Grove</t>
-  </si>
-  <si>
-    <t>Penguin Books</t>
-  </si>
-  <si>
-    <t>Sterling</t>
-  </si>
-  <si>
-    <t>Ed. Destino</t>
-  </si>
-  <si>
-    <t>A. H. Payne</t>
-  </si>
-  <si>
-    <t>Birken</t>
-  </si>
-  <si>
-    <t>Musées nationaux</t>
-  </si>
-  <si>
-    <t>Gallimard</t>
-  </si>
-  <si>
-    <t>Brooks/Cole</t>
-  </si>
-  <si>
-    <t>The @picture of Dorian Gray</t>
-  </si>
-  <si>
-    <t>Gustav Klimt - Art Nouveau visionary</t>
-  </si>
-  <si>
-    <t>La @familia de Pascual Duarte</t>
-  </si>
-  <si>
-    <t>eng</t>
-  </si>
-  <si>
-    <t>spa</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
@@ -256,12 +187,6 @@
     <t>8</t>
   </si>
   <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>LS1|FMAG|LS1|7/029|FMAG|FMAG|FMAG|7/029|FMAG|FMAG</t>
   </si>
   <si>
@@ -271,12 +196,6 @@
     <t>BBK-ROM|BBK-ROM|BBK-ROM|BBK-ROM|BBK-ROM</t>
   </si>
   <si>
-    <t>HG-MAG</t>
-  </si>
-  <si>
-    <t>BBK-ROM|BBK-ROM|BBK-ROM|LS1</t>
-  </si>
-  <si>
     <t>https://opac.sub.uni-goettingen.de/DB=1/SET=2/TTL=1/CMD?ACT=SRCHA&amp;IKT=1016&amp;SRT=YOP&amp;TRM=tit The picture of Dorian Gray&amp;MATCFILTER=N&amp;MATCSET=N&amp;NOSCAN=N&amp;ADI_BIB=</t>
   </si>
   <si>
@@ -286,21 +205,6 @@
     <t>https://opac.sub.uni-goettingen.de/DB=1/SET=2/TTL=1/CMD?ACT=SRCHA&amp;IKT=1016&amp;SRT=YOP&amp;TRM=tit La familia de Pascual Duarte&amp;MATCFILTER=N&amp;MATCSET=N&amp;NOSCAN=N&amp;ADI_BIB=</t>
   </si>
   <si>
-    <t>https://opac.sub.uni-goettingen.de/DB=1/SET=2/TTL=1/CMD?ACT=SRCHA&amp;IKT=1016&amp;SRT=YOP&amp;TRM=tit Auf der Eidechsburg&amp;MATCFILTER=N&amp;MATCSET=N&amp;NOSCAN=N&amp;ADI_BIB=</t>
-  </si>
-  <si>
-    <t>https://opac.sub.uni-goettingen.de/DB=1/SET=2/TTL=1/CMD?ACT=SRCHA&amp;IKT=1016&amp;SRT=YOP&amp;TRM=tit Bayerisches Kochbuch&amp;MATCFILTER=N&amp;MATCSET=N&amp;NOSCAN=N&amp;ADI_BIB=</t>
-  </si>
-  <si>
-    <t>https://opac.sub.uni-goettingen.de/DB=1/SET=2/TTL=1/CMD?ACT=SRCHA&amp;IKT=1016&amp;SRT=YOP&amp;TRM=tit Centenaire de l‘Impressionisme&amp;MATCFILTER=N&amp;MATCSET=N&amp;NOSCAN=N&amp;ADI_BIB=</t>
-  </si>
-  <si>
-    <t>https://opac.sub.uni-goettingen.de/DB=1/SET=2/TTL=1/CMD?ACT=SRCHA&amp;IKT=1016&amp;SRT=YOP&amp;TRM=tit Les parents terribles&amp;MATCFILTER=N&amp;MATCSET=N&amp;NOSCAN=N&amp;ADI_BIB=</t>
-  </si>
-  <si>
-    <t>https://opac.sub.uni-goettingen.de/DB=1/SET=2/TTL=1/CMD?ACT=SRCHA&amp;IKT=1016&amp;SRT=YOP&amp;TRM=tit Straightforward Statistics&amp;MATCFILTER=N&amp;MATCSET=N&amp;NOSCAN=N&amp;ADI_BIB=</t>
-  </si>
-  <si>
     <t>29</t>
   </si>
   <si>
@@ -320,21 +224,6 @@
   </si>
   <si>
     <t>https://opac.sub.uni-goettingen.de/DB=1/SET=2/TTL=1/CMD?ACT=SRCHA&amp;IKT=1016&amp;SRT=YOP&amp;TRM=TIT"La familia de Pascual Duarte" and PER Cela&amp;MATCFILTER=N&amp;MATCSET=N&amp;NOSCAN=N&amp;ADI_BIB=</t>
-  </si>
-  <si>
-    <t>https://opac.sub.uni-goettingen.de/DB=1/SET=2/TTL=1/CMD?ACT=SRCHA&amp;IKT=1016&amp;SRT=YOP&amp;TRM=TIT"Auf der Eidechsburg" and PER Tanner&amp;MATCFILTER=N&amp;MATCSET=N&amp;NOSCAN=N&amp;ADI_BIB=</t>
-  </si>
-  <si>
-    <t>https://opac.sub.uni-goettingen.de/DB=1/SET=2/TTL=1/CMD?ACT=SRCHA&amp;IKT=1016&amp;SRT=YOP&amp;TRM=TIT"Bayerisches Kochbuch" and PER Hofmann&amp;MATCFILTER=N&amp;MATCSET=N&amp;NOSCAN=N&amp;ADI_BIB=</t>
-  </si>
-  <si>
-    <t>https://opac.sub.uni-goettingen.de/DB=1/SET=2/TTL=1/CMD?ACT=SRCHA&amp;IKT=1016&amp;SRT=YOP&amp;TRM=TIT"Centenaire de l‘Impressionisme" and PER &amp;MATCFILTER=N&amp;MATCSET=N&amp;NOSCAN=N&amp;ADI_BIB=</t>
-  </si>
-  <si>
-    <t>https://opac.sub.uni-goettingen.de/DB=1/SET=2/TTL=1/CMD?ACT=SRCHA&amp;IKT=1016&amp;SRT=YOP&amp;TRM=TIT"Les parents terribles" and PER Cocteau&amp;MATCFILTER=N&amp;MATCSET=N&amp;NOSCAN=N&amp;ADI_BIB=</t>
-  </si>
-  <si>
-    <t>https://opac.sub.uni-goettingen.de/DB=1/SET=2/TTL=1/CMD?ACT=SRCHA&amp;IKT=1016&amp;SRT=YOP&amp;TRM=TIT"Straightforward Statistics" and PER Evans&amp;MATCFILTER=N&amp;MATCSET=N&amp;NOSCAN=N&amp;ADI_BIB=</t>
   </si>
 </sst>
 </file>
@@ -705,7 +594,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y9"/>
+  <dimension ref="A1:Y4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -793,70 +682,70 @@
         <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="E2" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="F2" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="G2" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="H2" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="I2" t="s">
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="J2" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="K2">
         <v>3</v>
       </c>
       <c r="L2">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M2">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="N2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="P2">
         <v>0</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="R2" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="S2" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="T2">
         <v>8</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>87</v>
+        <v>60</v>
       </c>
       <c r="V2" t="s">
-        <v>95</v>
+        <v>63</v>
       </c>
       <c r="W2" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="X2">
         <v>9</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>99</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:25">
@@ -867,22 +756,22 @@
         <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="F3" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="G3" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="H3" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="I3" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="J3" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="K3">
         <v>2</v>
@@ -891,31 +780,31 @@
         <v>212</v>
       </c>
       <c r="N3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="P3">
         <v>0</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="R3" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="S3" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="T3">
         <v>1</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>88</v>
+        <v>61</v>
       </c>
       <c r="X3">
         <v>0</v>
       </c>
       <c r="Y3" s="2" t="s">
-        <v>100</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:25">
@@ -926,28 +815,28 @@
         <v>26</v>
       </c>
       <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" t="s">
         <v>33</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" t="s">
         <v>39</v>
       </c>
-      <c r="E4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F4" t="s">
-        <v>50</v>
-      </c>
-      <c r="G4" t="s">
-        <v>54</v>
-      </c>
       <c r="H4" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="I4" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="J4" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
       <c r="K4">
         <v>2</v>
@@ -959,284 +848,40 @@
         <v>162</v>
       </c>
       <c r="N4" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="O4" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="P4">
         <v>0</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="R4" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="S4" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="T4">
         <v>0</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>89</v>
+        <v>62</v>
       </c>
       <c r="V4" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="W4" t="s">
-        <v>98</v>
+        <v>66</v>
       </c>
       <c r="X4">
         <v>0</v>
       </c>
       <c r="Y4" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G5" t="s">
-        <v>55</v>
-      </c>
-      <c r="H5" t="s">
-        <v>62</v>
-      </c>
-      <c r="L5">
-        <v>1</v>
-      </c>
-      <c r="M5">
-        <v>1</v>
-      </c>
-      <c r="R5" t="s">
-        <v>51</v>
-      </c>
-      <c r="T5">
-        <v>0</v>
-      </c>
-      <c r="U5" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="V5" t="s">
-        <v>51</v>
-      </c>
-      <c r="X5">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6">
-        <v>1950</v>
-      </c>
-      <c r="F6" t="s">
-        <v>51</v>
-      </c>
-      <c r="G6" t="s">
-        <v>56</v>
-      </c>
-      <c r="H6" t="s">
-        <v>63</v>
-      </c>
-      <c r="L6">
-        <v>41</v>
-      </c>
-      <c r="M6">
-        <v>22</v>
-      </c>
-      <c r="R6" t="s">
-        <v>72</v>
-      </c>
-      <c r="S6" t="s">
-        <v>85</v>
-      </c>
-      <c r="T6">
-        <v>0</v>
-      </c>
-      <c r="U6" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="V6" t="s">
-        <v>51</v>
-      </c>
-      <c r="X6">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7">
-        <v>1974</v>
-      </c>
-      <c r="F7" t="s">
-        <v>51</v>
-      </c>
-      <c r="G7" t="s">
-        <v>57</v>
-      </c>
-      <c r="H7" t="s">
-        <v>64</v>
-      </c>
-      <c r="L7">
-        <v>6</v>
-      </c>
-      <c r="R7" t="s">
-        <v>51</v>
-      </c>
-      <c r="T7">
-        <v>0</v>
-      </c>
-      <c r="U7" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="X7">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E8">
-        <v>1938</v>
-      </c>
-      <c r="F8" t="s">
-        <v>51</v>
-      </c>
-      <c r="G8" t="s">
-        <v>57</v>
-      </c>
-      <c r="H8" t="s">
-        <v>65</v>
-      </c>
-      <c r="L8">
-        <v>107</v>
-      </c>
-      <c r="M8">
-        <v>98</v>
-      </c>
-      <c r="R8" t="s">
-        <v>80</v>
-      </c>
-      <c r="S8" t="s">
-        <v>86</v>
-      </c>
-      <c r="T8">
-        <v>1</v>
-      </c>
-      <c r="U8" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="V8" t="s">
-        <v>80</v>
-      </c>
-      <c r="W8" t="s">
-        <v>86</v>
-      </c>
-      <c r="X8">
-        <v>1</v>
-      </c>
-      <c r="Y8" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9">
-        <v>1996</v>
-      </c>
-      <c r="F9" t="s">
-        <v>51</v>
-      </c>
-      <c r="G9" t="s">
-        <v>58</v>
-      </c>
-      <c r="H9" t="s">
-        <v>66</v>
-      </c>
-      <c r="L9">
-        <v>32</v>
-      </c>
-      <c r="R9" t="s">
-        <v>81</v>
-      </c>
-      <c r="T9">
-        <v>0</v>
-      </c>
-      <c r="U9" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="V9" t="s">
-        <v>51</v>
-      </c>
-      <c r="X9">
-        <v>0</v>
-      </c>
-      <c r="Y9" s="2" t="s">
-        <v>106</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1250,16 +895,6 @@
     <hyperlink ref="Q4" r:id="rId7"/>
     <hyperlink ref="U4" r:id="rId8"/>
     <hyperlink ref="Y4" r:id="rId9"/>
-    <hyperlink ref="U5" r:id="rId10"/>
-    <hyperlink ref="Y5" r:id="rId11"/>
-    <hyperlink ref="U6" r:id="rId12"/>
-    <hyperlink ref="Y6" r:id="rId13"/>
-    <hyperlink ref="U7" r:id="rId14"/>
-    <hyperlink ref="Y7" r:id="rId15"/>
-    <hyperlink ref="U8" r:id="rId16"/>
-    <hyperlink ref="Y8" r:id="rId17"/>
-    <hyperlink ref="U9" r:id="rId18"/>
-    <hyperlink ref="Y9" r:id="rId19"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
small changes in funcionts
</commit_message>
<xml_diff>
--- a/data/output/Anfragen_Geschenk_Muster_Spendende_Beispiele.xlsx
+++ b/data/output/Anfragen_Geschenk_Muster_Spendende_Beispiele.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="102">
   <si>
     <t>Titel</t>
   </si>
@@ -31,18 +31,18 @@
     <t>ISBN</t>
   </si>
   <si>
+    <t>Erscheinungsort</t>
+  </si>
+  <si>
+    <t>Verlag</t>
+  </si>
+  <si>
     <t>nach_ISBN_Titel</t>
   </si>
   <si>
     <t>nach_ISBN_Sprache_Text</t>
   </si>
   <si>
-    <t>Verlag</t>
-  </si>
-  <si>
-    <t>Erscheinungsort</t>
-  </si>
-  <si>
     <t>nach_ISBN_Bestand_K10</t>
   </si>
   <si>
@@ -55,10 +55,7 @@
     <t>nach_ISBN_Bestand_Göttingen</t>
   </si>
   <si>
-    <t>nach_ISBN_Ort_SUB</t>
-  </si>
-  <si>
-    <t>nach_ISBN_Bestand_SUB</t>
+    <t>nach_ISBN_Ort_Göttingen</t>
   </si>
   <si>
     <t>nach_ISBN_URL_GUK</t>
@@ -67,10 +64,7 @@
     <t>nach_Titel_Bestand_Göttingen</t>
   </si>
   <si>
-    <t>nach_Titel_Ort_SUB</t>
-  </si>
-  <si>
-    <t>nach_Titel_Bestand_SUB</t>
+    <t>nach_Titel_Ort_Göttingen</t>
   </si>
   <si>
     <t>nach_Titel_URL_GUK</t>
@@ -79,10 +73,7 @@
     <t>nach_Titel_Nachname_Autor_Bestand_Göttingen</t>
   </si>
   <si>
-    <t>nach_Titel_Nachname_Autor_Ort_SUB</t>
-  </si>
-  <si>
-    <t>nach_Titel_Nachname_Autor_Bestand_SUB</t>
+    <t>nach_Titel_Nachname_Autor_Ort_Göttingen</t>
   </si>
   <si>
     <t>nach_Titel_Nachname_Autor_URL_GUK</t>
@@ -97,18 +88,57 @@
     <t>La familia de Pascual Duarte</t>
   </si>
   <si>
+    <t>Auf der Eidechsburg</t>
+  </si>
+  <si>
+    <t>Bayerisches Kochbuch</t>
+  </si>
+  <si>
+    <t>Centenaire de l‘Impressionisme</t>
+  </si>
+  <si>
+    <t>Les parents terribles</t>
+  </si>
+  <si>
+    <t>Straightforward Statistics</t>
+  </si>
+  <si>
     <t>Oscar</t>
   </si>
   <si>
     <t>Camilo José</t>
   </si>
   <si>
+    <t>Ilse-Dore</t>
+  </si>
+  <si>
+    <t>Maria</t>
+  </si>
+  <si>
+    <t>Jean</t>
+  </si>
+  <si>
+    <t>James D.</t>
+  </si>
+  <si>
     <t>Wilde</t>
   </si>
   <si>
     <t>Cela</t>
   </si>
   <si>
+    <t>Tanner</t>
+  </si>
+  <si>
+    <t>Hofmann</t>
+  </si>
+  <si>
+    <t>Cocteau</t>
+  </si>
+  <si>
+    <t>Evans</t>
+  </si>
+  <si>
     <t>1994</t>
   </si>
   <si>
@@ -118,6 +148,9 @@
     <t>2009</t>
   </si>
   <si>
+    <t>1938?</t>
+  </si>
+  <si>
     <t>9780140623222</t>
   </si>
   <si>
@@ -127,6 +160,54 @@
     <t>9788423339044</t>
   </si>
   <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>New York [u.a.]</t>
+  </si>
+  <si>
+    <t>Barcelona</t>
+  </si>
+  <si>
+    <t>Leipzig</t>
+  </si>
+  <si>
+    <t>München</t>
+  </si>
+  <si>
+    <t>Paris</t>
+  </si>
+  <si>
+    <t>Pacific Grove</t>
+  </si>
+  <si>
+    <t>Penguin Books</t>
+  </si>
+  <si>
+    <t>Sterling</t>
+  </si>
+  <si>
+    <t>Ed. Destino</t>
+  </si>
+  <si>
+    <t>A. H. Payne</t>
+  </si>
+  <si>
+    <t>Birken</t>
+  </si>
+  <si>
+    <t>Musées nationaux</t>
+  </si>
+  <si>
+    <t>Gallimard</t>
+  </si>
+  <si>
+    <t>Brooks/Cole</t>
+  </si>
+  <si>
     <t>The @picture of Dorian Gray</t>
   </si>
   <si>
@@ -142,31 +223,13 @@
     <t>spa</t>
   </si>
   <si>
-    <t>Penguin Books</t>
-  </si>
-  <si>
-    <t>Sterling</t>
-  </si>
-  <si>
-    <t>Ed. Destino</t>
-  </si>
-  <si>
-    <t>London</t>
-  </si>
-  <si>
-    <t>New York [u.a.]</t>
-  </si>
-  <si>
-    <t>Barcelona</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
-    <t>BBK-ROM</t>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>['BBK-ROM']</t>
   </si>
   <si>
     <t>https://opac.sub.uni-goettingen.de/DB=1/SET=6/TTL=1/CMD?ACT=SRCHA&amp;IKT=1016&amp;SRT=YOP&amp;TRM=isb+9780140623222&amp;MATCFILTER=N&amp;MATCSET=N&amp;NOSCAN=N&amp;ADI_BIB=</t>
@@ -187,13 +250,22 @@
     <t>8</t>
   </si>
   <si>
-    <t>LS1|FMAG|LS1|7/029|FMAG|FMAG|FMAG|7/029|FMAG|FMAG</t>
-  </si>
-  <si>
-    <t>7/055|7/055|LS1|BBW-KJL</t>
-  </si>
-  <si>
-    <t>BBK-ROM|BBK-ROM|BBK-ROM|BBK-ROM|BBK-ROM</t>
+    <t>4</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>['7/029', 'FMAG', 'LS1']</t>
+  </si>
+  <si>
+    <t>['7/055', 'BBW-KJL', 'LS1']</t>
+  </si>
+  <si>
+    <t>['HG-MAG']</t>
+  </si>
+  <si>
+    <t>['BBK-ROM', 'LS1']</t>
   </si>
   <si>
     <t>https://opac.sub.uni-goettingen.de/DB=1/SET=2/TTL=1/CMD?ACT=SRCHA&amp;IKT=1016&amp;SRT=YOP&amp;TRM=tit The picture of Dorian Gray&amp;MATCFILTER=N&amp;MATCSET=N&amp;NOSCAN=N&amp;ADI_BIB=</t>
@@ -205,18 +277,27 @@
     <t>https://opac.sub.uni-goettingen.de/DB=1/SET=2/TTL=1/CMD?ACT=SRCHA&amp;IKT=1016&amp;SRT=YOP&amp;TRM=tit La familia de Pascual Duarte&amp;MATCFILTER=N&amp;MATCSET=N&amp;NOSCAN=N&amp;ADI_BIB=</t>
   </si>
   <si>
+    <t>https://opac.sub.uni-goettingen.de/DB=1/SET=2/TTL=1/CMD?ACT=SRCHA&amp;IKT=1016&amp;SRT=YOP&amp;TRM=tit Auf der Eidechsburg&amp;MATCFILTER=N&amp;MATCSET=N&amp;NOSCAN=N&amp;ADI_BIB=</t>
+  </si>
+  <si>
+    <t>https://opac.sub.uni-goettingen.de/DB=1/SET=2/TTL=1/CMD?ACT=SRCHA&amp;IKT=1016&amp;SRT=YOP&amp;TRM=tit Bayerisches Kochbuch&amp;MATCFILTER=N&amp;MATCSET=N&amp;NOSCAN=N&amp;ADI_BIB=</t>
+  </si>
+  <si>
+    <t>https://opac.sub.uni-goettingen.de/DB=1/SET=2/TTL=1/CMD?ACT=SRCHA&amp;IKT=1016&amp;SRT=YOP&amp;TRM=tit Centenaire de l‘Impressionisme&amp;MATCFILTER=N&amp;MATCSET=N&amp;NOSCAN=N&amp;ADI_BIB=</t>
+  </si>
+  <si>
+    <t>https://opac.sub.uni-goettingen.de/DB=1/SET=2/TTL=1/CMD?ACT=SRCHA&amp;IKT=1016&amp;SRT=YOP&amp;TRM=tit Les parents terribles&amp;MATCFILTER=N&amp;MATCSET=N&amp;NOSCAN=N&amp;ADI_BIB=</t>
+  </si>
+  <si>
+    <t>https://opac.sub.uni-goettingen.de/DB=1/SET=2/TTL=1/CMD?ACT=SRCHA&amp;IKT=1016&amp;SRT=YOP&amp;TRM=tit Straightforward Statistics&amp;MATCFILTER=N&amp;MATCSET=N&amp;NOSCAN=N&amp;ADI_BIB=</t>
+  </si>
+  <si>
     <t>29</t>
   </si>
   <si>
     <t>5</t>
   </si>
   <si>
-    <t>LS1|LS1|7/029|FMAG|FMAG|7/029|FMAG|FMAG|FMAG|LS1|7/029|FMAG</t>
-  </si>
-  <si>
-    <t>BBK-ROM|BBK-ROM|BBK-ROM|BBK-ROM</t>
-  </si>
-  <si>
     <t>https://opac.sub.uni-goettingen.de/DB=1/SET=2/TTL=1/CMD?ACT=SRCHA&amp;IKT=1016&amp;SRT=YOP&amp;TRM=TIT"The picture of Dorian Gray" and PER Wilde&amp;MATCFILTER=N&amp;MATCSET=N&amp;NOSCAN=N&amp;ADI_BIB=</t>
   </si>
   <si>
@@ -224,6 +305,21 @@
   </si>
   <si>
     <t>https://opac.sub.uni-goettingen.de/DB=1/SET=2/TTL=1/CMD?ACT=SRCHA&amp;IKT=1016&amp;SRT=YOP&amp;TRM=TIT"La familia de Pascual Duarte" and PER Cela&amp;MATCFILTER=N&amp;MATCSET=N&amp;NOSCAN=N&amp;ADI_BIB=</t>
+  </si>
+  <si>
+    <t>https://opac.sub.uni-goettingen.de/DB=1/SET=2/TTL=1/CMD?ACT=SRCHA&amp;IKT=1016&amp;SRT=YOP&amp;TRM=TIT"Auf der Eidechsburg" and PER Tanner&amp;MATCFILTER=N&amp;MATCSET=N&amp;NOSCAN=N&amp;ADI_BIB=</t>
+  </si>
+  <si>
+    <t>https://opac.sub.uni-goettingen.de/DB=1/SET=2/TTL=1/CMD?ACT=SRCHA&amp;IKT=1016&amp;SRT=YOP&amp;TRM=TIT"Bayerisches Kochbuch" and PER Hofmann&amp;MATCFILTER=N&amp;MATCSET=N&amp;NOSCAN=N&amp;ADI_BIB=</t>
+  </si>
+  <si>
+    <t>https://opac.sub.uni-goettingen.de/DB=1/SET=2/TTL=1/CMD?ACT=SRCHA&amp;IKT=1016&amp;SRT=YOP&amp;TRM=TIT"Centenaire de l‘Impressionisme" and PER &amp;MATCFILTER=N&amp;MATCSET=N&amp;NOSCAN=N&amp;ADI_BIB=</t>
+  </si>
+  <si>
+    <t>https://opac.sub.uni-goettingen.de/DB=1/SET=2/TTL=1/CMD?ACT=SRCHA&amp;IKT=1016&amp;SRT=YOP&amp;TRM=TIT"Les parents terribles" and PER Cocteau&amp;MATCFILTER=N&amp;MATCSET=N&amp;NOSCAN=N&amp;ADI_BIB=</t>
+  </si>
+  <si>
+    <t>https://opac.sub.uni-goettingen.de/DB=1/SET=2/TTL=1/CMD?ACT=SRCHA&amp;IKT=1016&amp;SRT=YOP&amp;TRM=TIT"Straightforward Statistics" and PER Evans&amp;MATCFILTER=N&amp;MATCSET=N&amp;NOSCAN=N&amp;ADI_BIB=</t>
   </si>
 </sst>
 </file>
@@ -594,13 +690,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y4"/>
+  <dimension ref="A1:V9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:22">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -664,46 +760,37 @@
       <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>23</v>
-      </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:22">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E2" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="F2" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="G2" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="H2" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="I2" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="J2" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="K2">
         <v>3</v>
@@ -717,61 +804,55 @@
       <c r="N2" t="s">
         <v>48</v>
       </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>51</v>
+      <c r="O2" t="s">
+        <v>70</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>75</v>
       </c>
       <c r="R2" t="s">
-        <v>54</v>
-      </c>
-      <c r="S2" t="s">
-        <v>57</v>
-      </c>
-      <c r="T2">
-        <v>8</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="V2" t="s">
-        <v>63</v>
-      </c>
-      <c r="W2" t="s">
-        <v>65</v>
-      </c>
-      <c r="X2">
-        <v>9</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>67</v>
+        <v>80</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="T2" t="s">
+        <v>92</v>
+      </c>
+      <c r="U2" t="s">
+        <v>80</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:22">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="F3" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="G3" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="H3" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="I3" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="J3" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="K3">
         <v>2</v>
@@ -782,61 +863,58 @@
       <c r="N3" t="s">
         <v>48</v>
       </c>
-      <c r="P3">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>52</v>
+      <c r="O3" t="s">
+        <v>70</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>76</v>
       </c>
       <c r="R3" t="s">
-        <v>55</v>
-      </c>
-      <c r="S3" t="s">
-        <v>58</v>
-      </c>
-      <c r="T3">
-        <v>1</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="X3">
-        <v>0</v>
-      </c>
-      <c r="Y3" s="2" t="s">
-        <v>68</v>
+        <v>81</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="U3" t="s">
+        <v>70</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:22">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="F4" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="G4" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="H4" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="I4" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="J4" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="K4">
         <v>2</v>
@@ -848,53 +926,289 @@
         <v>162</v>
       </c>
       <c r="N4" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="O4" t="s">
-        <v>50</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>77</v>
+      </c>
+      <c r="R4" t="s">
+        <v>71</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="T4" t="s">
+        <v>93</v>
+      </c>
+      <c r="U4" t="s">
+        <v>71</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H5" t="s">
+        <v>59</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>48</v>
+      </c>
+      <c r="R5" t="s">
+        <v>70</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="T5" t="s">
+        <v>48</v>
+      </c>
+      <c r="U5" t="s">
+        <v>70</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6">
+        <v>1950</v>
+      </c>
+      <c r="F6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" t="s">
         <v>53</v>
       </c>
-      <c r="R4" t="s">
-        <v>56</v>
-      </c>
-      <c r="S4" t="s">
-        <v>59</v>
-      </c>
-      <c r="T4">
-        <v>0</v>
-      </c>
-      <c r="U4" s="2" t="s">
+      <c r="H6" t="s">
+        <v>60</v>
+      </c>
+      <c r="L6">
+        <v>41</v>
+      </c>
+      <c r="M6">
+        <v>22</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>69</v>
+      </c>
+      <c r="R6" t="s">
+        <v>82</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="T6" t="s">
+        <v>48</v>
+      </c>
+      <c r="U6" t="s">
+        <v>70</v>
+      </c>
+      <c r="V6" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7">
+        <v>1974</v>
+      </c>
+      <c r="F7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7" t="s">
+        <v>54</v>
+      </c>
+      <c r="H7" t="s">
+        <v>61</v>
+      </c>
+      <c r="L7">
+        <v>6</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>48</v>
+      </c>
+      <c r="R7" t="s">
+        <v>70</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="U7" t="s">
+        <v>70</v>
+      </c>
+      <c r="V7" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8">
+        <v>1938</v>
+      </c>
+      <c r="F8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" t="s">
+        <v>54</v>
+      </c>
+      <c r="H8" t="s">
         <v>62</v>
       </c>
-      <c r="V4" t="s">
-        <v>64</v>
-      </c>
-      <c r="W4" t="s">
-        <v>66</v>
-      </c>
-      <c r="X4">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="2" t="s">
-        <v>69</v>
+      <c r="L8">
+        <v>107</v>
+      </c>
+      <c r="M8">
+        <v>98</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>78</v>
+      </c>
+      <c r="R8" t="s">
+        <v>83</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="T8" t="s">
+        <v>78</v>
+      </c>
+      <c r="U8" t="s">
+        <v>83</v>
+      </c>
+      <c r="V8" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9">
+        <v>1996</v>
+      </c>
+      <c r="F9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" t="s">
+        <v>55</v>
+      </c>
+      <c r="H9" t="s">
+        <v>63</v>
+      </c>
+      <c r="L9">
+        <v>32</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>79</v>
+      </c>
+      <c r="R9" t="s">
+        <v>70</v>
+      </c>
+      <c r="S9" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="T9" t="s">
+        <v>48</v>
+      </c>
+      <c r="U9" t="s">
+        <v>70</v>
+      </c>
+      <c r="V9" s="2" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="Q2" r:id="rId1"/>
-    <hyperlink ref="U2" r:id="rId2"/>
-    <hyperlink ref="Y2" r:id="rId3"/>
-    <hyperlink ref="Q3" r:id="rId4"/>
-    <hyperlink ref="U3" r:id="rId5"/>
-    <hyperlink ref="Y3" r:id="rId6"/>
-    <hyperlink ref="Q4" r:id="rId7"/>
-    <hyperlink ref="U4" r:id="rId8"/>
-    <hyperlink ref="Y4" r:id="rId9"/>
+    <hyperlink ref="P2" r:id="rId1"/>
+    <hyperlink ref="S2" r:id="rId2"/>
+    <hyperlink ref="V2" r:id="rId3"/>
+    <hyperlink ref="P3" r:id="rId4"/>
+    <hyperlink ref="S3" r:id="rId5"/>
+    <hyperlink ref="V3" r:id="rId6"/>
+    <hyperlink ref="P4" r:id="rId7"/>
+    <hyperlink ref="S4" r:id="rId8"/>
+    <hyperlink ref="V4" r:id="rId9"/>
+    <hyperlink ref="S5" r:id="rId10"/>
+    <hyperlink ref="V5" r:id="rId11"/>
+    <hyperlink ref="S6" r:id="rId12"/>
+    <hyperlink ref="V6" r:id="rId13"/>
+    <hyperlink ref="S7" r:id="rId14"/>
+    <hyperlink ref="V7" r:id="rId15"/>
+    <hyperlink ref="S8" r:id="rId16"/>
+    <hyperlink ref="V8" r:id="rId17"/>
+    <hyperlink ref="S9" r:id="rId18"/>
+    <hyperlink ref="V9" r:id="rId19"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>